<commit_message>
notes till 12th july
</commit_message>
<xml_diff>
--- a/Questions/after 2 days problems.xlsx
+++ b/Questions/after 2 days problems.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Scaler\Scaler Notes + Questions List\Questions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEC299BD-05FD-4AC2-B7CC-55FBB5CAEA3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98CF5D76-60DF-4D11-8B57-9217D3761A0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t xml:space="preserve">Question </t>
   </si>
@@ -48,13 +48,22 @@
   </si>
   <si>
     <t>solve before</t>
+  </si>
+  <si>
+    <t>Kth Symbol - Hard</t>
+  </si>
+  <si>
+    <t>Mod Sum</t>
+  </si>
+  <si>
+    <t>Largest Coprime Divisor</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -66,6 +75,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -88,14 +105,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="1">
@@ -131,8 +152,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8F14F630-C35A-4C67-89EE-A5030B04F6D4}" name="Table2" displayName="Table2" ref="D4:F5" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="D4:F5" xr:uid="{8F14F630-C35A-4C67-89EE-A5030B04F6D4}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8F14F630-C35A-4C67-89EE-A5030B04F6D4}" name="Table2" displayName="Table2" ref="D4:F7" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="D4:F7" xr:uid="{8F14F630-C35A-4C67-89EE-A5030B04F6D4}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{E414DB8E-94BC-4AC1-BBFD-22124B7E15B4}" name="S.no"/>
     <tableColumn id="2" xr3:uid="{AF4B9A71-0ED9-4B0D-8B30-18EF98906AB7}" name="Question "/>
@@ -405,10 +426,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="D4:F4"/>
+  <dimension ref="D4:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -430,10 +451,48 @@
         <v>2</v>
       </c>
     </row>
+    <row r="5" spans="4:6" x14ac:dyDescent="0.35">
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" s="3">
+        <v>45486</v>
+      </c>
+    </row>
+    <row r="6" spans="4:6" x14ac:dyDescent="0.35">
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" s="3">
+        <v>45487</v>
+      </c>
+    </row>
+    <row r="7" spans="4:6" x14ac:dyDescent="0.35">
+      <c r="D7">
+        <v>3</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F7" s="3">
+        <v>45487</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E5" r:id="rId1" display="https://www.scaler.com/academy/mentee-dashboard/class/236233/homework/problems/31788?navref=cl_tt_lst_nm" xr:uid="{42A78B15-0CF9-4891-8ACC-6D4456733716}"/>
+    <hyperlink ref="E6" r:id="rId2" display="https://www.scaler.com/academy/mentee-dashboard/class/236267/assignment/problems/4745?navref=cl_tt_lst_nm" xr:uid="{5723599F-2887-4F98-BF28-A1D5B84F4890}"/>
+    <hyperlink ref="E7" r:id="rId3" display="https://www.scaler.com/academy/mentee-dashboard/class/236267/homework/problems/358?navref=cl_tt_lst_nm" xr:uid="{FA821698-3480-412F-837D-2AB84AA06B6F}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>